<commit_message>
Handled singleton uncontested races
</commit_message>
<xml_diff>
--- a/data/extracted/Congressional Election Results by State (2008 - 111th).xlsx
+++ b/data/extracted/Congressional Election Results by State (2008 - 111th).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/ushouse/data/extracted/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CD5F54-2444-7442-B3AB-C639626AF9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E46F9B-5222-DA4D-8021-638BF701D3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="500" windowWidth="22400" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -570,7 +570,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -592,6 +592,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -657,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -764,6 +770,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2021,7 +2028,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:E54" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -2736,10 +2743,10 @@
   <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3:I52"/>
+      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3007,7 +3014,7 @@
       <c r="I6" s="82">
         <v>1</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="83">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4942,7 +4949,7 @@
       <c r="I47" s="82">
         <v>0</v>
       </c>
-      <c r="J47" s="21">
+      <c r="J47" s="83">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>

</xml_diff>